<commit_message>
Parallel seed 25 no_iit and iit_no_mod --> output results
</commit_message>
<xml_diff>
--- a/results/MLP_parallel/s_MLP_parallel_data_insilico_seed_25_2025-02-08_PH_30/output.xlsx
+++ b/results/MLP_parallel/s_MLP_parallel_data_insilico_seed_25_2025-02-08_PH_30/output.xlsx
@@ -511,25 +511,25 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>0.00568203</t>
+          <t>0.029253814</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>0.056641914</t>
+          <t>0.079765536</t>
         </is>
       </c>
       <c r="D3" t="n">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F3" t="n">
         <v>0</v>
       </c>
       <c r="G3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H3" t="n">
         <v>0</v>
@@ -571,19 +571,19 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>0.020217307</t>
+          <t>0.019499771</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>0.10839062</t>
+          <t>0.10570555</t>
         </is>
       </c>
       <c r="D5" t="n">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F5" t="n">
         <v>0</v>

</xml_diff>